<commit_message>
[FIX] pca phylum scientific names [WILDCARD] A bag of magic beans.
</commit_message>
<xml_diff>
--- a/resources/report.xlsx
+++ b/resources/report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/Papers/bit analysis/bit-analysis/comparative_func_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/Papers/bit analysis/bit-analysis/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_24018149414BBABF6410B4D55F5DCE3A87478EFA" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9F98E864-3CF6-4E03-967E-2886B7948E80}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_24018149414BBABF6410B4D55F5DCE3A87478EFA" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0DB6BB0E-0CBF-4FD1-AFD7-3E0F5E243823}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1311,11 +1311,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">

</xml_diff>